<commit_message>
I think this one saved safely.
-Inseok 1/16
</commit_message>
<xml_diff>
--- a/Project Backlog.xlsx
+++ b/Project Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Features</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,19 +38,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Example 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Example 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Example 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Example 4</t>
+    <t>Login button transitions to login screen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M3-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M3-2</t>
+  </si>
+  <si>
+    <t>Login Screen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Welcome Page with Login/Register Buttons</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M3-3</t>
+  </si>
+  <si>
+    <t>M4-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Login Handling through Login Screen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M5-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Registration Handling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Registration Screen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M5-2</t>
+  </si>
+  <si>
+    <t>M6-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Account Creation Screen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Account Creation Handling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M6-2</t>
+  </si>
+  <si>
+    <t>sdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Home Page Screen with Appropirate Buttons</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -97,12 +149,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,114 +460,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.625" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="12.375" customWidth="1"/>
-    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="43.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1">
         <v>1</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="1">
         <v>2</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I1" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>0.3</v>
+      </c>
+      <c r="E2">
+        <f>C2*(1+D2)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>0.2</v>
+      </c>
+      <c r="E3">
+        <f>C3*(1+D3)</f>
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
         <v>0.3</v>
       </c>
-      <c r="D2">
-        <f>B2*(1+C2)</f>
+      <c r="E4">
+        <f>C4*(1+D4)</f>
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>0.3</v>
+      </c>
+      <c r="E8">
+        <f>C8*(1+D8)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C3">
-        <v>0.2</v>
-      </c>
-      <c r="D3">
-        <f>B3*(1+C3)</f>
-        <v>16.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>0.3</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D5" si="0">B4*(1+C4)</f>
-        <v>19.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="C5">
-        <v>0.3</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <f>SUM(B2:B5)</f>
-        <v>59</v>
-      </c>
-      <c r="D6">
-        <f>SUM(D2:D5)</f>
-        <v>75.3</v>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished naming all the features for the project. Not sure if I made it too vague or not. Would appreciate someone else taking a look at the Project Backlog.xlsx.
</commit_message>
<xml_diff>
--- a/Project Backlog.xlsx
+++ b/Project Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Features</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,11 +98,83 @@
     <t>M6-2</t>
   </si>
   <si>
-    <t>sdf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Home Page Screen with Appropirate Buttons</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M6-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M7-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Account Selection Screen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Account Balance Screen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Transaction Screen with Appropriate Fields</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Transaction Handling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M7-2</t>
+  </si>
+  <si>
+    <t>M7-3</t>
+  </si>
+  <si>
+    <t>M7-4</t>
+  </si>
+  <si>
+    <t>M8-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spending Category Report Screen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spending Category Report Promt Screen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M8-2</t>
+  </si>
+  <si>
+    <t>M9-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Save/Loading Application</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M9-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local Information Storage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code Documentations</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -460,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -509,15 +581,9 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>0.3</v>
-      </c>
       <c r="E2">
         <f>C2*(1+D2)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -527,15 +593,9 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>14</v>
-      </c>
-      <c r="D3">
-        <v>0.2</v>
-      </c>
       <c r="E3">
         <f>C3*(1+D3)</f>
-        <v>16.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -545,15 +605,9 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>0.3</v>
-      </c>
       <c r="E4">
         <f>C4*(1+D4)</f>
-        <v>19.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -563,6 +617,10 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
+      <c r="E6">
+        <f>C6*(1+D6)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -571,15 +629,9 @@
       <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
-        <v>20</v>
-      </c>
-      <c r="D8">
-        <v>0.3</v>
-      </c>
       <c r="E8">
         <f>C8*(1+D8)</f>
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -589,16 +641,21 @@
       <c r="B9" t="s">
         <v>14</v>
       </c>
+      <c r="E9">
+        <f>C9*(1+D9)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
         <v>21</v>
+      </c>
+      <c r="E11">
+        <f>C11*(1+D11)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -608,10 +665,154 @@
       <c r="B12" t="s">
         <v>18</v>
       </c>
+      <c r="E12">
+        <f>C12*(1+D12)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
       <c r="B13" t="s">
         <v>19</v>
+      </c>
+      <c r="E13">
+        <f>C13*(1+D13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15">
+        <f>C15*(1+D15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <f>C16*(1+D16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17">
+        <f>C17*(1+D17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18">
+        <f>C18*(1+D18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20">
+        <f>C20*(1+D20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21">
+        <f>C21*(1+D21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23">
+        <f>C23*(1+D23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24">
+        <f>C24*(1+D24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26">
+        <f>C26*(1+D26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28">
+        <f>SUM(C2:C27)</f>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f>SUM(E2:E27)</f>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f>SUM(G2:G27)</f>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f>SUM(H2:H27)</f>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f>SUM(I2:I27)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Might as well upload these. These are the ones I've turned in Friday.
-Inseok Hwang
</commit_message>
<xml_diff>
--- a/Project Backlog.xlsx
+++ b/Project Backlog.xlsx
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -581,9 +581,15 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>0.3</v>
+      </c>
       <c r="E2">
         <f>C2*(1+D2)</f>
-        <v>0</v>
+        <v>7.8000000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -593,9 +599,15 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>0.3</v>
+      </c>
       <c r="E3">
         <f>C3*(1+D3)</f>
-        <v>0</v>
+        <v>7.8000000000000007</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -605,9 +617,15 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>0.3</v>
+      </c>
       <c r="E4">
         <f>C4*(1+D4)</f>
-        <v>0</v>
+        <v>7.8000000000000007</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -617,9 +635,15 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>0.3</v>
+      </c>
       <c r="E6">
         <f>C6*(1+D6)</f>
-        <v>0</v>
+        <v>7.8000000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -629,9 +653,15 @@
       <c r="B8" t="s">
         <v>15</v>
       </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>0.3</v>
+      </c>
       <c r="E8">
         <f>C8*(1+D8)</f>
-        <v>0</v>
+        <v>7.8000000000000007</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -641,9 +671,15 @@
       <c r="B9" t="s">
         <v>14</v>
       </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>0.3</v>
+      </c>
       <c r="E9">
         <f>C9*(1+D9)</f>
-        <v>0</v>
+        <v>7.8000000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -653,9 +689,15 @@
       <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>0.3</v>
+      </c>
       <c r="E11">
         <f>C11*(1+D11)</f>
-        <v>0</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -665,9 +707,15 @@
       <c r="B12" t="s">
         <v>18</v>
       </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>0.3</v>
+      </c>
       <c r="E12">
         <f>C12*(1+D12)</f>
-        <v>0</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -677,9 +725,15 @@
       <c r="B13" t="s">
         <v>19</v>
       </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>0.3</v>
+      </c>
       <c r="E13">
         <f>C13*(1+D13)</f>
-        <v>0</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -689,9 +743,15 @@
       <c r="B15" t="s">
         <v>24</v>
       </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>0.3</v>
+      </c>
       <c r="E15">
         <f>C15*(1+D15)</f>
-        <v>0</v>
+        <v>3.9000000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -701,9 +761,15 @@
       <c r="B16" t="s">
         <v>25</v>
       </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>0.3</v>
+      </c>
       <c r="E16">
         <f>C16*(1+D16)</f>
-        <v>0</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -713,9 +779,15 @@
       <c r="B17" t="s">
         <v>26</v>
       </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>0.3</v>
+      </c>
       <c r="E17">
         <f>C17*(1+D17)</f>
-        <v>0</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -725,9 +797,15 @@
       <c r="B18" t="s">
         <v>27</v>
       </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>0.3</v>
+      </c>
       <c r="E18">
         <f>C18*(1+D18)</f>
-        <v>0</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -737,9 +815,15 @@
       <c r="B20" t="s">
         <v>33</v>
       </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>0.3</v>
+      </c>
       <c r="E20">
         <f>C20*(1+D20)</f>
-        <v>0</v>
+        <v>7.8000000000000007</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -749,9 +833,15 @@
       <c r="B21" t="s">
         <v>32</v>
       </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>0.3</v>
+      </c>
       <c r="E21">
         <f>C21*(1+D21)</f>
-        <v>0</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -761,9 +851,15 @@
       <c r="B23" t="s">
         <v>36</v>
       </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>0.3</v>
+      </c>
       <c r="E23">
         <f>C23*(1+D23)</f>
-        <v>0</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -773,9 +869,15 @@
       <c r="B24" t="s">
         <v>38</v>
       </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>0.3</v>
+      </c>
       <c r="E24">
         <f>C24*(1+D24)</f>
-        <v>0</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -785,9 +887,15 @@
       <c r="B26" t="s">
         <v>40</v>
       </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>0.3</v>
+      </c>
       <c r="E26">
         <f>C26*(1+D26)</f>
-        <v>0</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -796,11 +904,14 @@
       </c>
       <c r="C28">
         <f>SUM(C2:C27)</f>
-        <v>0</v>
+        <v>97</v>
+      </c>
+      <c r="D28">
+        <v>0.3</v>
       </c>
       <c r="E28">
         <f>SUM(E2:E27)</f>
-        <v>0</v>
+        <v>126.10000000000004</v>
       </c>
       <c r="G28">
         <f>SUM(G2:G27)</f>

</xml_diff>